<commit_message>
added missing cal events, assigned OOI bar codes where necessary, corrected integration events
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA05MOAS-GL493_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA05MOAS-GL493_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\# OOI_Asset_Management\GA_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="6720" windowWidth="27120" windowHeight="10356" tabRatio="377"/>
+    <workbookView xWindow="5520" yWindow="6720" windowWidth="27120" windowHeight="10350" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Ref Des</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>N00408</t>
+  </si>
+  <si>
+    <t>OL000108</t>
+  </si>
+  <si>
+    <t>GL493 Controller</t>
   </si>
 </sst>
 </file>
@@ -787,26 +793,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="29.6640625" customWidth="1"/>
-    <col min="13" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" customWidth="1"/>
+    <col min="13" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
@@ -844,7 +850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -886,11 +892,11 @@
         <v>-42.455928333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
@@ -909,24 +915,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -952,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -981,7 +987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1077,7 +1083,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1110,7 +1116,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1143,7 +1149,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -1156,16 +1162,18 @@
       <c r="D11" s="9">
         <v>2</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9">
-        <v>493</v>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
       </c>
       <c r="G11" s="9"/>
       <c r="I11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>

</xml_diff>

<commit_message>
added recovered dates to global MOAS
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA05MOAS-GL493_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA05MOAS-GL493_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="6720" windowWidth="27120" windowHeight="10350" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="5520" yWindow="6720" windowWidth="27120" windowHeight="10360" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$104</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -547,7 +542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,7 +577,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,26 +788,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
-    <col min="13" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" customWidth="1"/>
+    <col min="13" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="42">
       <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
@@ -850,7 +845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="15">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -869,7 +864,9 @@
       <c r="F2" s="8">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7">
+        <v>42321</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>21</v>
       </c>
@@ -892,11 +889,11 @@
         <v>-42.455928333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
@@ -915,24 +912,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="13" customFormat="1" ht="28">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -958,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -987,7 +984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1016,7 +1013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1045,7 +1042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1074,7 +1071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1083,7 +1080,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="3" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1116,7 +1113,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="3" customFormat="1">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -1140,7 +1137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="3" customFormat="1">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1149,7 +1146,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="3" customFormat="1">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -1173,7 +1170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="3" customFormat="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>

</xml_diff>

<commit_message>
updated Water Depth for global MOAS
Open Ocean Gliders: Water Depth = 1000
Global Profiling Gliders: Water Depth = 200
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA05MOAS-GL493_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA05MOAS-GL493_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="6720" windowWidth="27120" windowHeight="10360" tabRatio="377"/>
+    <workbookView xWindow="39600" yWindow="6620" windowWidth="27120" windowHeight="10360" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$104</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -874,7 +874,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="6">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>28</v>

</xml_diff>